<commit_message>
Improve BLE characteristic details
</commit_message>
<xml_diff>
--- a/documentation/commandDetails.xlsx
+++ b/documentation/commandDetails.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25502"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDAF5D1B-9639-4024-85BB-2D52736E88D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8264656A-5FA5-4F48-B885-E95CF5A33387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLE characteristics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
   <si>
     <t>Service</t>
   </si>
@@ -75,25 +75,55 @@
     <t>tar_curr</t>
   </si>
   <si>
-    <t>4 byte array. Float referring to target value of DC stim. Little endian format.</t>
+    <t>4 byte array. Float referring to target value of DC stim, current. Little endian format.</t>
   </si>
   <si>
     <t>base_curr</t>
   </si>
   <si>
-    <t>4 byte array. Float referring to base value of DC stim. Little endian format.</t>
+    <t>4 byte array. Float referring to base value of DC stim, current. Little endian format.</t>
   </si>
   <si>
     <t>timing</t>
   </si>
   <si>
-    <t>8 byte array. 4 sets of 2 bytes, each set in little endian format.</t>
+    <t>12 byte array. 3 sets of 4 bytes, each in little endian format. Order: Slope, Flat, Interstim</t>
   </si>
   <si>
     <t>pulses</t>
   </si>
   <si>
+    <t>4 byte array. Little endian uint32_t. Number of pulses we are aiming to complete with DC</t>
+  </si>
+  <si>
     <t>burst_serv</t>
+  </si>
+  <si>
+    <t>4 byte array. Little endian uint32_t</t>
+  </si>
+  <si>
+    <t>bursts</t>
+  </si>
+  <si>
+    <t>p1_curr</t>
+  </si>
+  <si>
+    <t>4 byte array. Little endian float giving current of phase 1</t>
+  </si>
+  <si>
+    <t>p2_curr</t>
+  </si>
+  <si>
+    <t>4 byte array. Little endian float giving current of phase 2</t>
+  </si>
+  <si>
+    <t>anodic</t>
+  </si>
+  <si>
+    <t>1 byte array. 1 if anodic, 0 if not.</t>
+  </si>
+  <si>
+    <t>20 byte array. 5 sets of 4 bytes, each set in little endian format. Order: Interstim, P1, Interphase, P2, Interburst</t>
   </si>
   <si>
     <t>Command</t>
@@ -643,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,7 +684,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -748,13 +778,80 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -766,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5351FB22-414C-4B7F-902F-DEF68C6AD228}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -779,291 +876,291 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>